<commit_message>
updated EM02 formater file.
</commit_message>
<xml_diff>
--- a/EM02.xlsx
+++ b/EM02.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test\Documents\GitHub\report-generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dheeraj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5087C48-8AD6-4303-AFE0-0684518F3BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFD79AF-F4B1-4612-A9F1-3751A255FFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Unique</t>
   </si>
@@ -48,30 +57,12 @@
     <t>Open</t>
   </si>
   <si>
-    <t>LGT1_yahoo_Open</t>
-  </si>
-  <si>
-    <t>Link01_yahoo_Open</t>
-  </si>
-  <si>
-    <t>MKT_yahoo_Open</t>
-  </si>
-  <si>
     <t>Unique_Open_Total</t>
   </si>
   <si>
     <t>Click</t>
   </si>
   <si>
-    <t>LGT1_yahoo_Click</t>
-  </si>
-  <si>
-    <t>Link01_yahoo_Click</t>
-  </si>
-  <si>
-    <t>MKT_yahoo_Click</t>
-  </si>
-  <si>
     <t>Unique_Click_Total</t>
   </si>
   <si>
@@ -90,27 +81,9 @@
     <t>Dup_Raw_Total</t>
   </si>
   <si>
-    <t>Dup_LGT1_Open</t>
-  </si>
-  <si>
-    <t>Dup_Link1_Open</t>
-  </si>
-  <si>
-    <t>Dup_Mkt_Open</t>
-  </si>
-  <si>
     <t>Dup_Open_Total</t>
   </si>
   <si>
-    <t>Dup_LGT1_Click</t>
-  </si>
-  <si>
-    <t>Dup_Link1_Click</t>
-  </si>
-  <si>
-    <t>Dup_Mkt_Click</t>
-  </si>
-  <si>
     <t>Dup_Click_Total</t>
   </si>
   <si>
@@ -178,6 +151,45 @@
   </si>
   <si>
     <t>Dup_MKT_Raw</t>
+  </si>
+  <si>
+    <t>Link1_Unique_Opn_yh</t>
+  </si>
+  <si>
+    <t>MKT_Unique_Opn_Yh</t>
+  </si>
+  <si>
+    <t>LGT1_Unique_Opn_yh</t>
+  </si>
+  <si>
+    <t>Link1_Unique_Clk_yh</t>
+  </si>
+  <si>
+    <t>MKT_Unique_Clk_Yh</t>
+  </si>
+  <si>
+    <t>LGT1_Unique_Clk_yh</t>
+  </si>
+  <si>
+    <t>MKT_Dupe_Opn_yh</t>
+  </si>
+  <si>
+    <t>LGT1_Dupe_Opn_Yh</t>
+  </si>
+  <si>
+    <t>Link1_Dupe_Opn_yh</t>
+  </si>
+  <si>
+    <t>MKT_Dupe_Clk_yh</t>
+  </si>
+  <si>
+    <t>LGT1_Dupe_Clk_Yh</t>
+  </si>
+  <si>
+    <t>Link1_Dupe_Clk_yh</t>
+  </si>
+  <si>
+    <t> 61821</t>
   </si>
 </sst>
 </file>
@@ -341,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -370,9 +382,6 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -657,97 +666,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M22:M23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="17" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="17" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="18" t="s">
         <v>31</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>43</v>
       </c>
       <c r="N1" s="18" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="S1" s="17" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="T1" s="17" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="U1" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45544</v>
       </c>
@@ -763,8 +772,8 @@
       <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="23">
-        <v>61821</v>
+      <c r="I2" t="s">
+        <v>51</v>
       </c>
       <c r="R2" s="19" t="e">
         <f t="shared" ref="R2:S28" si="0">N2/M2</f>
@@ -783,7 +792,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45544</v>
       </c>
@@ -799,7 +808,7 @@
       <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3">
         <v>61824</v>
       </c>
       <c r="R3" s="19" t="e">
@@ -819,7 +828,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45544</v>
       </c>
@@ -835,7 +844,7 @@
       <c r="G4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4">
         <v>61827</v>
       </c>
       <c r="R4" s="19" t="e">
@@ -855,7 +864,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45544</v>
       </c>
@@ -867,8 +876,6 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
       <c r="J5" s="6">
         <f t="shared" ref="J5:Q5" si="3">SUM(J2:J4)</f>
         <v>0</v>
@@ -918,7 +925,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45544</v>
       </c>
@@ -932,9 +939,9 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="23">
+        <v>39</v>
+      </c>
+      <c r="I6">
         <v>61822</v>
       </c>
       <c r="R6" s="19" t="e">
@@ -954,7 +961,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45544</v>
       </c>
@@ -968,9 +975,9 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="23">
+        <v>40</v>
+      </c>
+      <c r="I7">
         <v>61825</v>
       </c>
       <c r="R7" s="19" t="e">
@@ -990,7 +997,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45544</v>
       </c>
@@ -1004,9 +1011,9 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="23">
+        <v>41</v>
+      </c>
+      <c r="I8">
         <v>61828</v>
       </c>
       <c r="R8" s="19" t="e">
@@ -1026,20 +1033,18 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45544</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
       <c r="J9" s="6">
         <f t="shared" ref="J9:Q9" si="4">SUM(J6:J8)</f>
         <v>0</v>
@@ -1089,7 +1094,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45544</v>
       </c>
@@ -1097,15 +1102,15 @@
         <v>0</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="23">
+        <v>42</v>
+      </c>
+      <c r="I10">
         <v>61823</v>
       </c>
       <c r="R10" s="19" t="e">
@@ -1125,7 +1130,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45544</v>
       </c>
@@ -1133,15 +1138,15 @@
         <v>0</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="23">
+        <v>43</v>
+      </c>
+      <c r="I11">
         <v>61826</v>
       </c>
       <c r="R11" s="19" t="e">
@@ -1161,7 +1166,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45544</v>
       </c>
@@ -1169,15 +1174,15 @@
         <v>0</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="23">
+        <v>44</v>
+      </c>
+      <c r="I12">
         <v>61829</v>
       </c>
       <c r="R12" s="19" t="e">
@@ -1197,20 +1202,18 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45544</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
       <c r="J13" s="6">
         <f t="shared" ref="J13:Q13" si="5">SUM(J10:J12)</f>
         <v>0</v>
@@ -1260,7 +1263,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45544</v>
       </c>
@@ -1268,12 +1271,10 @@
       <c r="C14" s="10"/>
       <c r="D14" s="5"/>
       <c r="E14" s="10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
       <c r="J14" s="6">
         <f t="shared" ref="J14:Q14" si="6">SUM(J13,J9,J5)</f>
         <v>0</v>
@@ -1323,12 +1324,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45544</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>1</v>
@@ -1337,9 +1338,9 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="23">
+        <v>38</v>
+      </c>
+      <c r="I15">
         <v>61812</v>
       </c>
       <c r="R15" s="19" t="e">
@@ -1359,12 +1360,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45544</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>1</v>
@@ -1373,9 +1374,9 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="23">
+        <v>12</v>
+      </c>
+      <c r="I16">
         <v>62039</v>
       </c>
       <c r="R16" s="19" t="e">
@@ -1395,12 +1396,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45544</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>1</v>
@@ -1409,9 +1410,9 @@
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="23">
+        <v>13</v>
+      </c>
+      <c r="I17">
         <v>61818</v>
       </c>
       <c r="R17" s="19" t="e">
@@ -1431,20 +1432,18 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45544</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
       <c r="J18" s="6">
         <f t="shared" ref="J18:Q18" si="7">SUM(J15:J17)</f>
         <v>0</v>
@@ -1494,12 +1493,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45544</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>6</v>
@@ -1508,9 +1507,9 @@
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="23">
+        <v>45</v>
+      </c>
+      <c r="I19">
         <v>61813</v>
       </c>
       <c r="R19" s="19" t="e">
@@ -1530,12 +1529,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45544</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>6</v>
@@ -1544,9 +1543,9 @@
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="23">
+        <v>46</v>
+      </c>
+      <c r="I20">
         <v>61816</v>
       </c>
       <c r="R20" s="19" t="e">
@@ -1566,12 +1565,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45544</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>6</v>
@@ -1580,9 +1579,9 @@
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="23">
+        <v>47</v>
+      </c>
+      <c r="I21">
         <v>61819</v>
       </c>
       <c r="R21" s="19" t="e">
@@ -1602,20 +1601,18 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45544</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="13" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
       <c r="J22" s="6">
         <f t="shared" ref="J22:Q22" si="8">SUM(J19:J21)</f>
         <v>0</v>
@@ -1665,23 +1662,23 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45544</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I23" s="23">
+        <v>48</v>
+      </c>
+      <c r="I23">
         <v>61814</v>
       </c>
       <c r="R23" s="19" t="e">
@@ -1701,23 +1698,23 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45544</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="23">
+        <v>49</v>
+      </c>
+      <c r="I24">
         <v>61817</v>
       </c>
       <c r="R24" s="19" t="e">
@@ -1737,23 +1734,23 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45544</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
       <c r="G25" t="s">
-        <v>26</v>
-      </c>
-      <c r="I25" s="23">
+        <v>50</v>
+      </c>
+      <c r="I25">
         <v>61820</v>
       </c>
       <c r="R25" s="19" t="e">
@@ -1773,20 +1770,18 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45544</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="13" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
       <c r="J26" s="6">
         <f t="shared" ref="J26:Q26" si="9">SUM(J23:J25)</f>
         <v>0</v>
@@ -1836,7 +1831,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45544</v>
       </c>
@@ -1844,12 +1839,10 @@
       <c r="C27" s="16"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
       <c r="J27" s="6">
         <f t="shared" ref="J27:Q27" si="10">SUM(J26,J22,J18)</f>
         <v>0</v>
@@ -1899,7 +1892,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45544</v>
       </c>
@@ -1908,11 +1901,9 @@
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
       <c r="J28" s="6">
         <f t="shared" ref="J28:Q28" si="11">SUM(J27,J14)</f>
         <v>0</v>

</xml_diff>

<commit_message>
silly mistake by dheeraj sir so i updated  em02 formater
</commit_message>
<xml_diff>
--- a/EM02.xlsx
+++ b/EM02.xlsx
@@ -5,36 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dheeraj\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test\Documents\GitHub\report-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFD79AF-F4B1-4612-A9F1-3751A255FFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0389FE42-0DB9-48D5-826A-31C212A59BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>Unique</t>
   </si>
@@ -187,9 +178,6 @@
   </si>
   <si>
     <t>Link1_Dupe_Clk_yh</t>
-  </si>
-  <si>
-    <t> 61821</t>
   </si>
 </sst>
 </file>
@@ -667,31 +655,31 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="17" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="17" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>19</v>
       </c>
@@ -756,7 +744,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45544</v>
       </c>
@@ -772,8 +760,8 @@
       <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" t="s">
-        <v>51</v>
+      <c r="I2">
+        <v>61821</v>
       </c>
       <c r="R2" s="19" t="e">
         <f t="shared" ref="R2:S28" si="0">N2/M2</f>
@@ -792,7 +780,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45544</v>
       </c>
@@ -828,7 +816,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45544</v>
       </c>
@@ -864,7 +852,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45544</v>
       </c>
@@ -925,7 +913,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45544</v>
       </c>
@@ -961,7 +949,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45544</v>
       </c>
@@ -997,7 +985,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45544</v>
       </c>
@@ -1033,7 +1021,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45544</v>
       </c>
@@ -1094,7 +1082,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45544</v>
       </c>
@@ -1130,7 +1118,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45544</v>
       </c>
@@ -1166,7 +1154,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45544</v>
       </c>
@@ -1202,7 +1190,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45544</v>
       </c>
@@ -1263,7 +1251,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45544</v>
       </c>
@@ -1324,7 +1312,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45544</v>
       </c>
@@ -1360,7 +1348,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45544</v>
       </c>
@@ -1396,7 +1384,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45544</v>
       </c>
@@ -1432,7 +1420,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45544</v>
       </c>
@@ -1493,7 +1481,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45544</v>
       </c>
@@ -1529,7 +1517,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45544</v>
       </c>
@@ -1565,7 +1553,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45544</v>
       </c>
@@ -1601,7 +1589,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45544</v>
       </c>
@@ -1662,7 +1650,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45544</v>
       </c>
@@ -1698,7 +1686,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45544</v>
       </c>
@@ -1734,7 +1722,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45544</v>
       </c>
@@ -1770,7 +1758,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45544</v>
       </c>
@@ -1831,7 +1819,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45544</v>
       </c>
@@ -1892,7 +1880,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45544</v>
       </c>

</xml_diff>